<commit_message>
Added images, corrected excel data, removed bbplot library call
</commit_message>
<xml_diff>
--- a/Demographic_summaries/data/MHS-demographic-info.xlsx
+++ b/Demographic_summaries/data/MHS-demographic-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\VT DSPG\R files\2021_DSPG_Loudoun\Demographic_summaries\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1769FFE7-F9E2-4F6D-9056-212E46818A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0342E36-0EBD-46A6-B49D-45E246198FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AAFA0FD7-4AC8-4A49-8385-7C16B800D06B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{AAFA0FD7-4AC8-4A49-8385-7C16B800D06B}"/>
   </bookViews>
   <sheets>
     <sheet name="Gender" sheetId="1" r:id="rId1"/>
@@ -519,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9123542C-0841-45B1-8A46-DEAB186FEA86}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -634,10 +634,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2962751-8383-443D-96B8-5A781BE86818}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -673,9 +673,8 @@
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2">
-        <f>B13/C13</f>
-        <v>4.5393858477970631E-2</v>
+      <c r="B2" s="6">
+        <v>34</v>
       </c>
       <c r="C2" s="6">
         <v>52</v>
@@ -701,8 +700,7 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <f>B14/C14</f>
-        <v>0.14819759679572764</v>
+        <v>111</v>
       </c>
       <c r="C3">
         <v>140</v>
@@ -727,9 +725,8 @@
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4">
-        <f>B15/C15</f>
-        <v>7.0761014686248333E-2</v>
+      <c r="B4" s="6">
+        <v>53</v>
       </c>
       <c r="C4" s="6">
         <v>54</v>
@@ -755,8 +752,7 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <f>B16/C16</f>
-        <v>4.0053404539385851E-3</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -781,9 +777,8 @@
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B6">
-        <f>B17/C17</f>
-        <v>0.1041388518024032</v>
+      <c r="B6" s="6">
+        <v>78</v>
       </c>
       <c r="C6" s="6">
         <v>84</v>
@@ -809,8 +804,7 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <f>B18/C18</f>
-        <v>3.2042723631508681E-2</v>
+        <v>24</v>
       </c>
       <c r="C7">
         <v>33</v>
@@ -835,9 +829,8 @@
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B8">
-        <f>B19/C19</f>
-        <v>0.59546061415220297</v>
+      <c r="B8" s="6">
+        <v>446</v>
       </c>
       <c r="C8" s="6">
         <v>440</v>
@@ -882,85 +875,6 @@
       </c>
       <c r="H9" s="9">
         <v>2839</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B13" s="6">
-        <v>34</v>
-      </c>
-      <c r="C13" s="9">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B14">
-        <v>111</v>
-      </c>
-      <c r="C14" s="9">
-        <v>749</v>
-      </c>
-      <c r="E14" s="6">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B15" s="6">
-        <v>53</v>
-      </c>
-      <c r="C15" s="9">
-        <v>749</v>
-      </c>
-      <c r="E15">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="C16" s="9">
-        <v>749</v>
-      </c>
-      <c r="E16" s="6">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B17" s="6">
-        <v>78</v>
-      </c>
-      <c r="C17" s="9">
-        <v>749</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B18">
-        <v>24</v>
-      </c>
-      <c r="C18" s="9">
-        <v>749</v>
-      </c>
-      <c r="E18" s="6">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B19" s="6">
-        <v>446</v>
-      </c>
-      <c r="C19" s="9">
-        <v>749</v>
-      </c>
-      <c r="E19">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="E20" s="6">
-        <v>440</v>
       </c>
     </row>
   </sheetData>

</xml_diff>